<commit_message>
Fixed file name typo, added additional placeholder to BOM
</commit_message>
<xml_diff>
--- a/Mechanical/Thinkpad 701C x Framework High Level BOM.xlsx
+++ b/Mechanical/Thinkpad 701C x Framework High Level BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl\Documents\KB Projects\Public\framework701c-repo\Mechanical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B17DD99-FAE4-456D-9FEB-7D0A28747D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF164352-77B8-4CD2-A8C7-14FC500DBD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19335" yWindow="2610" windowWidth="18030" windowHeight="15435" xr2:uid="{5BACC303-3B5E-4303-B7A5-10A6714632D6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
   <si>
     <t>Item</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>eDP adapter board screw</t>
+  </si>
+  <si>
+    <t>magnet for lid sensor</t>
   </si>
 </sst>
 </file>
@@ -556,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2159844B-1F48-4259-B5D6-2CA0580B4535}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,6 +1086,17 @@
         <v>56</v>
       </c>
     </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>